<commit_message>
updated crediting-notes translation table
</commit_message>
<xml_diff>
--- a/Notes-Crediting - Translation Table - Column DB.xlsx
+++ b/Notes-Crediting - Translation Table - Column DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Chloe\Judaica Digital Metadata Parser (JDMP)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canrongqiu/JDMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E162BF-6C50-4AD5-AB89-BE96DDB4C3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C47FE8-BEB3-3B47-BDFE-F5426FAC0D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F01FA83C-D28D-46BE-A10F-70EA2A7FB99C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{F01FA83C-D28D-46BE-A10F-70EA2A7FB99C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>231 Lowe</t>
   </si>
@@ -81,18 +80,33 @@
   </si>
   <si>
     <t>Digitization funded from the income of the Harvard-Littauer Judaica Endowment in the Harvard College Library (Fund 560153).</t>
+  </si>
+  <si>
+    <t>source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -141,7 +155,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -473,76 +487,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A3A69A-DDA0-481E-9F67-61880CDE3DF4}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="17.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="48">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" ht="48">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="48">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="48">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="48">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="48">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="48">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed country-code translation table + updated country handling
</commit_message>
<xml_diff>
--- a/Notes-Crediting - Translation Table - Column DB.xlsx
+++ b/Notes-Crediting - Translation Table - Column DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canrongqiu/JDMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C47FE8-BEB3-3B47-BDFE-F5426FAC0D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CDDB02-25F7-4A4B-9297-D15E74B1A7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{F01FA83C-D28D-46BE-A10F-70EA2A7FB99C}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>

</xml_diff>